<commit_message>
Criacao de CatTarTest e correcao de algs detalhes noutras classes
</commit_message>
<xml_diff>
--- a/Sprint 2/DailyScrum.xlsx
+++ b/Sprint 2/DailyScrum.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
   <si>
     <t>1- Whats
  been done</t>
@@ -166,6 +166,34 @@
   </si>
   <si>
     <t>implementar classes registarColaboradorcontroller e areaGestorUI</t>
+  </si>
+  <si>
+    <t>INICIADO INTERFACES GRAFICAS UC2E E IMPLEMENTACAO UC6</t>
+  </si>
+  <si>
+    <t>IMPLEMENTAR UI UC6</t>
+  </si>
+  <si>
+    <t>NADA A APONTAR</t>
+  </si>
+  <si>
+    <t>TERMINAR LIGACAO COM A API
+TERMINAR SERIALIZACAO DADOS</t>
+  </si>
+  <si>
+    <t>plano a - revisao javafx
+caso haja tempo trabalhar nas classes UI
+terminar uc1</t>
+  </si>
+  <si>
+    <t>terminar a areaColaboradorUI</t>
+  </si>
+  <si>
+    <t>CRIACAO CATEGORIATAREFA E CARACTERIZACAOCOMPTEC E RESPETIVO CONTROLLER
+PESQUISA CSS</t>
+  </si>
+  <si>
+    <t>FINALIZAR TDD CLASSES CRIADAS</t>
   </si>
 </sst>
 </file>
@@ -570,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -862,6 +890,76 @@
         <v>25</v>
       </c>
     </row>
+    <row r="25" spans="1:4" ht="163.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="6">
+        <v>44230</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="163.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="163.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="163.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="163.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -869,18 +967,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1042,18 +1140,25 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14B3AFF6-13C9-408E-8574-4783EB7A6A34}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BC044B2-0F43-479C-B8DA-0CF1CA3F78ED}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="8547ca18-4b18-44b0-ad77-125b4de67a73"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BC044B2-0F43-479C-B8DA-0CF1CA3F78ED}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14B3AFF6-13C9-408E-8574-4783EB7A6A34}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
finalized UC and SD
</commit_message>
<xml_diff>
--- a/Sprint 2/DailyScrum.xlsx
+++ b/Sprint 2/DailyScrum.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28705"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\victo\OneDrive\Ambiente de Trabalho\UpSkill\GitHub\upskill_java1_labprg_grupo3\Sprint 2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-440" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="0" yWindow="-444" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="63">
   <si>
     <t>1- Whats
  been done</t>
@@ -228,12 +233,23 @@
     <t>Rever Testes
 Atualizar Glossario
 Javadocs</t>
+  </si>
+  <si>
+    <t>atualização e conclusao dos artefactos de análise</t>
+  </si>
+  <si>
+    <t>testes de utilização da aplicação, ajuste de pequenos bugs e funcionalidades
+update da lógica mvc</t>
+  </si>
+  <si>
+    <t>testes de utilização da aplicação, ajuste de pequenos bugs e funcionalidades
+javadocs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -648,7 +664,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -656,19 +672,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
-    <col min="2" max="4" width="53.5" customWidth="1"/>
+    <col min="2" max="4" width="53.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="164.25" customHeight="1">
+    <row r="1" spans="1:4" ht="164.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6">
         <v>44224</v>
       </c>
@@ -682,7 +698,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="164.25" customHeight="1">
+    <row r="2" spans="1:4" ht="164.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -696,7 +712,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="164.5" customHeight="1">
+    <row r="3" spans="1:4" ht="164.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -710,7 +726,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="164.5" customHeight="1">
+    <row r="4" spans="1:4" ht="164.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -724,7 +740,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="164.5" customHeight="1">
+    <row r="5" spans="1:4" ht="164.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -738,7 +754,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="164.25" customHeight="1">
+    <row r="7" spans="1:4" ht="164.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>44225</v>
       </c>
@@ -752,7 +768,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="164.25" customHeight="1">
+    <row r="8" spans="1:4" ht="164.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -766,7 +782,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="164.25" customHeight="1">
+    <row r="9" spans="1:4" ht="164.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
@@ -780,7 +796,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="163.5" customHeight="1">
+    <row r="10" spans="1:4" ht="163.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -794,7 +810,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="164.25" customHeight="1">
+    <row r="11" spans="1:4" ht="164.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
@@ -808,7 +824,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="164.25" customHeight="1">
+    <row r="13" spans="1:4" ht="164.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>44228</v>
       </c>
@@ -822,7 +838,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="163.5" customHeight="1">
+    <row r="14" spans="1:4" ht="163.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -836,7 +852,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="162.75" customHeight="1">
+    <row r="15" spans="1:4" ht="162.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>4</v>
       </c>
@@ -850,7 +866,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="163.5" customHeight="1">
+    <row r="16" spans="1:4" ht="163.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>6</v>
       </c>
@@ -864,7 +880,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="164.25" customHeight="1">
+    <row r="17" spans="1:4" ht="164.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>5</v>
       </c>
@@ -878,7 +894,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="163.5" customHeight="1">
+    <row r="19" spans="1:4" ht="163.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>44229</v>
       </c>
@@ -892,7 +908,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="163.5" customHeight="1">
+    <row r="20" spans="1:4" ht="163.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
@@ -906,7 +922,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="163.5" customHeight="1">
+    <row r="21" spans="1:4" ht="163.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -920,7 +936,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="163.5" customHeight="1">
+    <row r="22" spans="1:4" ht="163.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>6</v>
       </c>
@@ -934,7 +950,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="163.5" customHeight="1">
+    <row r="23" spans="1:4" ht="163.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>5</v>
       </c>
@@ -948,7 +964,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="163.5" customHeight="1">
+    <row r="25" spans="1:4" ht="163.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
         <v>44230</v>
       </c>
@@ -962,7 +978,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="163.5" customHeight="1">
+    <row r="26" spans="1:4" ht="163.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>3</v>
       </c>
@@ -976,7 +992,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="163.5" customHeight="1">
+    <row r="27" spans="1:4" ht="163.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>4</v>
       </c>
@@ -990,7 +1006,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="163.5" customHeight="1">
+    <row r="28" spans="1:4" ht="163.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>6</v>
       </c>
@@ -1004,7 +1020,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="163.5" customHeight="1">
+    <row r="29" spans="1:4" ht="163.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>5</v>
       </c>
@@ -1018,7 +1034,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="89" customHeight="1">
+    <row r="31" spans="1:4" ht="88.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
         <v>44231</v>
       </c>
@@ -1032,7 +1048,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="167" customHeight="1">
+    <row r="32" spans="1:4" ht="166.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>3</v>
       </c>
@@ -1046,7 +1062,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="158" customHeight="1">
+    <row r="33" spans="1:4" ht="157.94999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>4</v>
       </c>
@@ -1060,7 +1076,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="206" customHeight="1">
+    <row r="34" spans="1:4" ht="205.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>6</v>
       </c>
@@ -1074,7 +1090,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="252" customHeight="1">
+    <row r="35" spans="1:4" ht="252" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>5</v>
       </c>
@@ -1085,6 +1101,76 @@
         <v>59</v>
       </c>
       <c r="D35" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="162.44999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="6">
+        <v>44232</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="162.44999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="162.44999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="162.44999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="162.44999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D41" s="7" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1100,21 +1186,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100E1596D6519E3454AA4F609AB910CDDB3" ma:contentTypeVersion="6" ma:contentTypeDescription="Criar um novo documento." ma:contentTypeScope="" ma:versionID="9b26b6fbb604c19d018ea2996a91ccd3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8547ca18-4b18-44b0-ad77-125b4de67a73" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f6e0f2b62ca9a86d6ed6d7e486c6920c" ns2:_="">
     <xsd:import namespace="8547ca18-4b18-44b0-ad77-125b4de67a73"/>
@@ -1272,31 +1343,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BC044B2-0F43-479C-B8DA-0CF1CA3F78ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="8547ca18-4b18-44b0-ad77-125b4de67a73"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14B3AFF6-13C9-408E-8574-4783EB7A6A34}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E07F5F7-E76B-45C3-9D63-EE965952A79F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1312,4 +1374,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14B3AFF6-13C9-408E-8574-4783EB7A6A34}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4BC044B2-0F43-479C-B8DA-0CF1CA3F78ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8547ca18-4b18-44b0-ad77-125b4de67a73"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>